<commit_message>
fixed some data and add some cuts
</commit_message>
<xml_diff>
--- a/datos/imagenes/Arturo/video-3/video-3.xlsx
+++ b/datos/imagenes/Arturo/video-3/video-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\notebooks\Paper interferometria\Interferometria - GUA\datos\imagenes\Arturo\video-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63095A7-E3CA-49B0-A1A3-3D65E38169D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3273BE15-0BD8-487E-9C6E-4666C44DA349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11676" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11256" yWindow="0" windowWidth="12072" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,29 +585,29 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>182</v>
+        <v>185.1</v>
       </c>
       <c r="E2" s="4">
-        <v>164.5</v>
+        <v>142.1</v>
       </c>
       <c r="F2" s="4">
-        <v>167.4</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="G2" s="5">
         <f>(E2+F2)/2</f>
-        <v>165.95</v>
+        <v>144.39999999999998</v>
       </c>
       <c r="H2" s="7">
         <f>(D2-G2)/(D2+G2)</f>
-        <v>4.6127317143267746E-2</v>
+        <v>0.12352048558421856</v>
       </c>
       <c r="I2" s="8">
         <f>AVERAGE(H2:H11)</f>
-        <v>8.0259947943757154E-2</v>
+        <v>9.3816378859325325E-2</v>
       </c>
       <c r="J2" s="8">
         <f>STDEVA(H2:H11)</f>
-        <v>3.7752715555518512E-2</v>
+        <v>3.1957153547527789E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -771,21 +771,21 @@
         <v>102</v>
       </c>
       <c r="D8" s="4">
-        <v>194.5</v>
+        <v>137.5</v>
       </c>
       <c r="E8" s="4">
-        <v>191.6</v>
+        <v>112.5</v>
       </c>
       <c r="F8" s="4">
-        <v>175</v>
+        <v>118.1</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>183.3</v>
+        <v>115.3</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="1"/>
-        <v>2.9645314981471646E-2</v>
+        <v>8.7816455696202542E-2</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>

</xml_diff>